<commit_message>
[docs] adicionando valores dos testes de funcionamento dos watermarks
</commit_message>
<xml_diff>
--- a/docs/formula_umidade.xlsx
+++ b/docs/formula_umidade.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreibosco/Devel/smartgreen/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreibosco/Devel/git/smartgreen/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="440" windowWidth="28760" windowHeight="18720"/>
+    <workbookView xWindow="13980" yWindow="460" windowWidth="13980" windowHeight="17560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t>Ta = (Rs-550)/137.5</t>
   </si>
@@ -132,6 +133,27 @@
   </si>
   <si>
     <t>http://www.emesystems.com/pdfs/SMX.pdf</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Bias</t>
+  </si>
+  <si>
+    <t>parece ainda estar umido</t>
+  </si>
+  <si>
+    <t>bias alto</t>
+  </si>
+  <si>
+    <t>ainda muito umido</t>
+  </si>
+  <si>
+    <t>ok (bias oscilando muito)</t>
   </si>
 </sst>
 </file>
@@ -163,12 +185,24 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -191,9 +225,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -512,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -563,7 +599,7 @@
         <v>1600</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B19" si="0">(A5-550)/137.5</f>
+        <f t="shared" ref="B5:B25" si="0">(A5-550)/137.5</f>
         <v>7.6363636363636367</v>
       </c>
       <c r="C5">
@@ -625,9 +661,12 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>845</v>
+      </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>-4</v>
+        <f>(A9-550)/137.5</f>
+        <v>2.1454545454545455</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -637,168 +676,885 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>366</v>
+      </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>-4</v>
+        <f>(A10-550)/137.5</f>
+        <v>-1.3381818181818181</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>745</v>
+      </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>-4</v>
+        <f>(A11-550)/137.5</f>
+        <v>1.4181818181818182</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>315</v>
+      </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>-4</v>
+        <f>(A12-550)/137.5</f>
+        <v>-1.709090909090909</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>685</v>
+      </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>-4</v>
+        <f>(A13-550)/137.5</f>
+        <v>0.98181818181818181</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>810</v>
+      </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>1.8909090909090909</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>704</v>
+      </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>705</v>
+      </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>1.1272727272727272</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>272</v>
+      </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-2.021818181818182</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>320</v>
+      </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-1.6727272727272726</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>202</v>
+      </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-2.5309090909090908</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>360</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>-1.3818181818181818</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
+      <c r="A21">
+        <v>490</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>-0.43636363636363634</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>334</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>-1.5709090909090908</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>312</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>-1.730909090909091</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>585</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.25454545454545452</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>421</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>-0.93818181818181823</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B27">
         <v>4700</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B28">
         <v>874</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B29">
         <v>693</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="1">
-        <f>(B21*(B22-B23)/B23)</f>
-        <v>1227.5613275613275</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>28</v>
+      <c r="A32" s="1">
+        <f>(B27*(B28-B29)/B29)</f>
+        <v>1227.5613275613275</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39">
-        <v>1.5</v>
-      </c>
-      <c r="B39">
-        <v>32</v>
-      </c>
-      <c r="C39">
-        <f>(3.213*A39+4.093)/(1-0.009733*A39-0.01205*B39)</f>
-        <v>14.859107319850517</v>
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>1.5</v>
+      </c>
+      <c r="B45">
+        <v>32</v>
+      </c>
+      <c r="C45">
+        <f>(3.213*A45+4.093)/(1-0.009733*A45-0.01205*B45)</f>
+        <v>14.859107319850517</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="B46">
+        <v>32</v>
+      </c>
+      <c r="C46">
+        <f>(3.213*A46+4.093)/(1-0.009733*A46-0.01205*B46)</f>
+        <v>11.19268288501239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1600</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B25" si="0">(A5-550)/137.5</f>
+        <v>7.6363636363636367</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>594</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>1100</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>845</v>
+      </c>
+      <c r="B9">
+        <f>(A9-550)/137.5</f>
+        <v>2.1454545454545455</v>
+      </c>
+      <c r="D9">
+        <f>(C9-550)/137.5</f>
+        <v>-4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>366</v>
+      </c>
+      <c r="B10">
+        <f>(A10-550)/137.5</f>
+        <v>-1.3381818181818181</v>
+      </c>
+      <c r="C10">
+        <v>1817</v>
+      </c>
+      <c r="D10">
+        <f>(C10-550)/137.5</f>
+        <v>9.2145454545454548</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10">
+        <v>-50</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>745</v>
+      </c>
+      <c r="B11">
+        <f>(A11-550)/137.5</f>
+        <v>1.4181818181818182</v>
+      </c>
+      <c r="C11">
+        <v>6426</v>
+      </c>
+      <c r="D11">
+        <f>(C11-550)/137.5</f>
+        <v>42.734545454545454</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>315</v>
+      </c>
+      <c r="B12">
+        <f>(A12-550)/137.5</f>
+        <v>-1.709090909090909</v>
+      </c>
+      <c r="C12">
+        <v>5870</v>
+      </c>
+      <c r="D12">
+        <f>(C12-550)/137.5</f>
+        <v>38.690909090909088</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>685</v>
+      </c>
+      <c r="B13">
+        <f>(A13-550)/137.5</f>
+        <v>0.98181818181818181</v>
+      </c>
+      <c r="C13">
+        <v>6129</v>
+      </c>
+      <c r="D13">
+        <f>(C13-550)/137.5</f>
+        <v>40.574545454545458</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>810</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1.8909090909090909</v>
+      </c>
+      <c r="C14">
+        <v>6966</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D25" si="1">(C14-550)/137.5</f>
+        <v>46.661818181818184</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>704</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C15">
+        <v>1900</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>9.8181818181818183</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>705</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>1.1272727272727272</v>
+      </c>
+      <c r="C16">
+        <v>1024</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>3.4472727272727273</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>272</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>-2.021818181818182</v>
+      </c>
+      <c r="C17">
+        <v>4330</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>27.490909090909092</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
+        <v>320</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.6727272727272726</v>
+      </c>
+      <c r="C18" s="2">
+        <v>730</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3090909090909091</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>202</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>-2.5309090909090908</v>
+      </c>
+      <c r="C19">
+        <v>2287</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>12.632727272727273</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
+        <v>360</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.3818181818181818</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3174</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="1"/>
+        <v>19.083636363636362</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="3">
+        <v>-267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>490</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>-0.43636363636363634</v>
+      </c>
+      <c r="C21">
+        <v>3472</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>21.25090909090909</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="2">
+        <v>334</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.5709090909090908</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1503</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
+        <v>6.9309090909090907</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="2">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>312</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>-1.730909090909091</v>
+      </c>
+      <c r="C23">
+        <v>4004</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>25.12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>585</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.25454545454545452</v>
+      </c>
+      <c r="C24">
+        <v>5613</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>36.82181818181818</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>421</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>-0.93818181818181823</v>
+      </c>
+      <c r="C25">
+        <v>5638</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>37.00363636363636</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
+        <f>(B27*(B28-B29)/B29)</f>
+        <v>1227.5613275613275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>1.5</v>
+      </c>
+      <c r="B45">
+        <v>32</v>
+      </c>
+      <c r="C45">
+        <f>(3.213*A45+4.093)/(1-0.009733*A45-0.01205*B45)</f>
+        <v>14.859107319850517</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="B46">
+        <v>32</v>
+      </c>
+      <c r="C46">
+        <f>(3.213*A46+4.093)/(1-0.009733*A46-0.01205*B46)</f>
+        <v>11.19268288501239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>